<commit_message>
Fix a typo in Excel Rate Ratios
</commit_message>
<xml_diff>
--- a/utilities/inst/Risk Group Rate Ratios for Tabby2.xlsx
+++ b/utilities/inst/Risk Group Rate Ratios for Tabby2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cht180/Documents/tabby2/utilities/inst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA111EAC-4CCC-B14D-AF50-91ABF2146477}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAAC6B83-E816-E840-B78D-2614696E8873}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21500" xr2:uid="{4EF77599-8302-3442-9ACA-0A10FE5EDA88}"/>
   </bookViews>
@@ -682,7 +682,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -721,7 +721,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="11">
-        <v>2.29</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D2" s="17">
         <v>1</v>
@@ -780,7 +780,7 @@
         <v>3.4</v>
       </c>
       <c r="D5" s="11">
-        <v>53</v>
+        <v>5.3</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>13</v>

</xml_diff>